<commit_message>
Add Prototype with lower Voltages
</commit_message>
<xml_diff>
--- a/circuit_sizing.xlsx
+++ b/circuit_sizing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\benedikt.schmidt\Entwicklung\dcconverter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE183CBC-6B8B-4776-B64F-4C35977A4843}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{452FBD2B-94AA-4057-9995-81288022C893}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{61C71F00-4B7F-4BCC-8214-45AF5950F01B}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{61C71F00-4B7F-4BCC-8214-45AF5950F01B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -139,8 +139,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A1EE8C96-04B5-4D62-83AC-7D8BB34E4A2C}" name="Table1" displayName="Table1" ref="A1:P7" totalsRowShown="0">
-  <autoFilter ref="A1:P7" xr:uid="{BBED3E59-775A-46B9-A106-ECCD63D733D7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A1EE8C96-04B5-4D62-83AC-7D8BB34E4A2C}" name="Table1" displayName="Table1" ref="A1:P8" totalsRowShown="0">
+  <autoFilter ref="A1:P8" xr:uid="{BBED3E59-775A-46B9-A106-ECCD63D733D7}"/>
   <tableColumns count="16">
     <tableColumn id="1" xr3:uid="{2CAF689D-0ABD-4BFA-A76B-154886D5A1B9}" name="Input Voltage [V]"/>
     <tableColumn id="2" xr3:uid="{54A549DF-AFF2-4354-84E1-A2D134D8F05B}" name="Output Voltage [V]"/>
@@ -478,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F13306D-DFB5-4F20-8916-FE70CCC0AD05}">
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,15 +564,15 @@
         <v>0.11360000000000001</v>
       </c>
       <c r="D2">
-        <f>B2*B2/C2</f>
+        <f t="shared" ref="D2:D7" si="0">B2*B2/C2</f>
         <v>220.07042253521126</v>
       </c>
       <c r="E2">
-        <f>C2/B2</f>
+        <f t="shared" ref="E2:E7" si="1">C2/B2</f>
         <v>2.2720000000000001E-2</v>
       </c>
       <c r="F2">
-        <f>A2/D2</f>
+        <f t="shared" ref="F2:F7" si="2">A2/D2</f>
         <v>0.22720000000000001</v>
       </c>
       <c r="G2" s="1">
@@ -592,23 +592,23 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <f>(100-K2)/100</f>
+        <f t="shared" ref="L2:L7" si="3">(100-K2)/100</f>
         <v>0.99</v>
       </c>
       <c r="M2">
-        <f>(-1)*H2/D2*LOG((A2-I2-B2)/(A2-I2-L2*B2),EXP(1))</f>
+        <f t="shared" ref="M2:M7" si="4">(-1)*H2/D2*LOG((A2-I2-B2)/(A2-I2-L2*B2),EXP(1))</f>
         <v>1.3997491535439439E-8</v>
       </c>
       <c r="N2">
-        <f>(-1)*H2/D2*LOG((J2+B2*L2)/(J2+B2),EXP(1))</f>
+        <f t="shared" ref="N2:N7" si="5">(-1)*H2/D2*LOG((J2+B2*L2)/(J2+B2),EXP(1))</f>
         <v>1.1255858765549513E-7</v>
       </c>
       <c r="O2">
-        <f>M2*1000000</f>
+        <f t="shared" ref="O2:P7" si="6">M2*1000000</f>
         <v>1.3997491535439438E-2</v>
       </c>
       <c r="P2">
-        <f>N2*1000000</f>
+        <f t="shared" si="6"/>
         <v>0.11255858765549513</v>
       </c>
     </row>
@@ -623,15 +623,15 @@
         <v>0.11360000000000001</v>
       </c>
       <c r="D3">
-        <f>B3*B3/C3</f>
+        <f t="shared" si="0"/>
         <v>220.07042253521126</v>
       </c>
       <c r="E3">
-        <f>C3/B3</f>
+        <f t="shared" si="1"/>
         <v>2.2720000000000001E-2</v>
       </c>
       <c r="F3">
-        <f>A3/D3</f>
+        <f t="shared" si="2"/>
         <v>4.5440000000000001E-2</v>
       </c>
       <c r="G3" s="1">
@@ -651,23 +651,23 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <f>(100-K3)/100</f>
+        <f t="shared" si="3"/>
         <v>0.99</v>
       </c>
       <c r="M3">
-        <f>(-1)*H3/D3*LOG((A3-I3-B3)/(A3-I3-L3*B3),EXP(1))</f>
+        <f t="shared" si="4"/>
         <v>1.6037875433353774E-7</v>
       </c>
       <c r="N3">
-        <f>(-1)*H3/D3*LOG((J3+B3*L3)/(J3+B3),EXP(1))</f>
+        <f t="shared" si="5"/>
         <v>1.1255858765549513E-7</v>
       </c>
       <c r="O3">
-        <f>M3*1000000</f>
+        <f t="shared" si="6"/>
         <v>0.16037875433353774</v>
       </c>
       <c r="P3">
-        <f>N3*1000000</f>
+        <f t="shared" si="6"/>
         <v>0.11255858765549513</v>
       </c>
     </row>
@@ -682,15 +682,15 @@
         <v>0.11360000000000001</v>
       </c>
       <c r="D4">
-        <f>B4*B4/C4</f>
+        <f t="shared" si="0"/>
         <v>220.07042253521126</v>
       </c>
       <c r="E4">
-        <f>C4/B4</f>
+        <f t="shared" si="1"/>
         <v>2.2720000000000001E-2</v>
       </c>
       <c r="F4">
-        <f>A4/D4</f>
+        <f t="shared" si="2"/>
         <v>4.5440000000000001E-2</v>
       </c>
       <c r="G4" s="1">
@@ -710,23 +710,23 @@
         <v>10</v>
       </c>
       <c r="L4">
-        <f>(100-K4)/100</f>
+        <f t="shared" si="3"/>
         <v>0.9</v>
       </c>
       <c r="M4">
-        <f>(-1)*H4/D4*LOG((A4-I4-B4)/(A4-I4-L4*B4),EXP(1))</f>
+        <f t="shared" si="4"/>
         <v>1.5165949029700968E-6</v>
       </c>
       <c r="N4">
-        <f>(-1)*H4/D4*LOG((J4+B4*L4)/(J4+B4),EXP(1))</f>
+        <f t="shared" si="5"/>
         <v>1.1749450051928328E-6</v>
       </c>
       <c r="O4">
-        <f>M4*1000000</f>
+        <f t="shared" si="6"/>
         <v>1.5165949029700969</v>
       </c>
       <c r="P4">
-        <f>N4*1000000</f>
+        <f t="shared" si="6"/>
         <v>1.1749450051928327</v>
       </c>
     </row>
@@ -741,15 +741,15 @@
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="D5">
-        <f>B5*B5/C5</f>
+        <f t="shared" si="0"/>
         <v>10000</v>
       </c>
       <c r="E5">
-        <f>C5/B5</f>
+        <f t="shared" si="1"/>
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="F5">
-        <f>A5/D5</f>
+        <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
       <c r="G5" s="1">
@@ -769,23 +769,23 @@
         <v>10</v>
       </c>
       <c r="L5">
-        <f>(100-K5)/100</f>
+        <f t="shared" si="3"/>
         <v>0.9</v>
       </c>
       <c r="M5">
-        <f>(-1)*H5/D5*LOG((A5-I5-B5)/(A5-I5-L5*B5),EXP(1))</f>
+        <f t="shared" si="4"/>
         <v>3.3375768111137697E-8</v>
       </c>
       <c r="N5">
-        <f>(-1)*H5/D5*LOG((J5+B5*L5)/(J5+B5),EXP(1))</f>
+        <f t="shared" si="5"/>
         <v>2.5857064374842273E-8</v>
       </c>
       <c r="O5">
-        <f>M5*1000000</f>
+        <f t="shared" si="6"/>
         <v>3.3375768111137696E-2</v>
       </c>
       <c r="P5">
-        <f>N5*1000000</f>
+        <f t="shared" si="6"/>
         <v>2.5857064374842274E-2</v>
       </c>
     </row>
@@ -800,15 +800,15 @@
         <v>2.5</v>
       </c>
       <c r="D6">
-        <f>B6*B6/C6</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="E6">
-        <f>C6/B6</f>
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
       <c r="F6">
-        <f>A6/D6</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G6" s="1">
@@ -828,23 +828,23 @@
         <v>10</v>
       </c>
       <c r="L6">
-        <f>(100-K6)/100</f>
+        <f t="shared" si="3"/>
         <v>0.9</v>
       </c>
       <c r="M6">
-        <f>(-1)*H6/D6*LOG((A6-I6-B6)/(A6-I6-L6*B6),EXP(1))</f>
+        <f t="shared" si="4"/>
         <v>3.3375768111137694E-5</v>
       </c>
       <c r="N6">
-        <f>(-1)*H6/D6*LOG((J6+B6*L6)/(J6+B6),EXP(1))</f>
+        <f t="shared" si="5"/>
         <v>2.5857064374842273E-5</v>
       </c>
       <c r="O6">
-        <f>M6*1000000</f>
+        <f t="shared" si="6"/>
         <v>33.375768111137695</v>
       </c>
       <c r="P6">
-        <f>N6*1000000</f>
+        <f t="shared" si="6"/>
         <v>25.857064374842274</v>
       </c>
     </row>
@@ -859,15 +859,15 @@
         <v>1</v>
       </c>
       <c r="D7">
-        <f>B7*B7/C7</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="E7">
-        <f>C7/B7</f>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="F7">
-        <f>A7/D7</f>
+        <f t="shared" si="2"/>
         <v>0.4</v>
       </c>
       <c r="G7" s="1">
@@ -899,12 +899,71 @@
         <v>4.3564159578761099E-5</v>
       </c>
       <c r="O7">
-        <f>M7*1000000</f>
+        <f t="shared" si="6"/>
         <v>50.460807855205104</v>
       </c>
       <c r="P7">
-        <f>N7*1000000</f>
+        <f t="shared" si="6"/>
         <v>43.5641595787611</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>20</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>0.32</v>
+      </c>
+      <c r="D8">
+        <f>B8*B8/C8</f>
+        <v>12.5</v>
+      </c>
+      <c r="E8">
+        <f>C8/B8</f>
+        <v>0.16</v>
+      </c>
+      <c r="F8">
+        <f>A8/D8</f>
+        <v>1.6</v>
+      </c>
+      <c r="G8" s="1">
+        <f>(Table1[[#This Row],[Input Voltage '[V']]]-Table1[[#This Row],[Forwared Voltage IGBT '[V']]])*Table1[[#This Row],[Load Current Constant On '[A']]]</f>
+        <v>30.080000000000002</v>
+      </c>
+      <c r="H8">
+        <v>5.4000000000000003E-3</v>
+      </c>
+      <c r="I8">
+        <v>1.2</v>
+      </c>
+      <c r="J8">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="K8">
+        <v>30</v>
+      </c>
+      <c r="L8">
+        <f>(100-K8)/100</f>
+        <v>0.7</v>
+      </c>
+      <c r="M8">
+        <f>(-1)*H8/D8*LOG((A8-I8-B8)/(A8-I8-L8*B8),EXP(1))</f>
+        <v>1.5159450158468715E-5</v>
+      </c>
+      <c r="N8">
+        <f>(-1)*H8/D8*LOG((J8+B8*L8)/(J8+B8),EXP(1))</f>
+        <v>1.1993691021045675E-4</v>
+      </c>
+      <c r="O8">
+        <f>M8*1000000</f>
+        <v>15.159450158468715</v>
+      </c>
+      <c r="P8">
+        <f>N8*1000000</f>
+        <v>119.93691021045676</v>
       </c>
     </row>
   </sheetData>

</xml_diff>